<commit_message>
Clean up of templates, incorporating dukes 5.1 into standard processing methods
</commit_message>
<xml_diff>
--- a/queens/config/templates/dukes_ch_1.xlsx
+++ b/queens/config/templates/dukes_ch_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\PycharmProjects\uk_energy_data_api\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro\AppData\Local\queens\queens\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6007FD23-1CA6-42F4-8738-B2FA04AC0003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950DBF3A-E358-47A3-B054-3087E90DCA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="12" xr2:uid="{C7A96D5D-A644-4012-B418-CE3BBCED0D4C}"/>
   </bookViews>
   <sheets>
     <sheet name="1.1" sheetId="10" r:id="rId1"/>
@@ -1689,15 +1689,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D05EE7-8D8D-45F8-9599-5A89EAB3B8C2}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -3066,13 +3067,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1026899-EDF0-43C7-8585-EB7C14354B18}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -3560,11 +3563,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9673C06D-0E7A-4BB1-9BEC-1A1D6219C856}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3645,11 +3654,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5005DDF-E2BC-4A3E-B667-90F5CBFB6BB1}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3730,13 +3745,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425282C-868D-490E-98D9-DD5403F8543C}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4262,15 +4279,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732E0C56-183C-4199-8E1E-44BA09BFCEE6}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="53.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5642,13 +5660,16 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -6875,16 +6896,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF71E3-D330-4248-A0E3-2256A1167A8F}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.77734375" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -8175,9 +8194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A95590D-4CE9-4A52-8AD4-52B5D68440D7}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8553,11 +8570,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D4341AC-9278-4308-B637-81E7010F9C46}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F1" sqref="C1:F1"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -8928,11 +8951,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F5497E-3E08-4F53-A7A4-FF5A523F6922}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D7:D8"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9051,11 +9078,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82253B5-151F-4D3E-BE53-1427E1059EE2}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -9192,13 +9223,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECFEABF-1827-41A5-9CBF-DD0F4CBE752D}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>